<commit_message>
Commit various log and config files
</commit_message>
<xml_diff>
--- a/alfred precision and recall from recent classifier runs_2020-06-09.xlsx
+++ b/alfred precision and recall from recent classifier runs_2020-06-09.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alfre\Code\jupyter\cs230_spring2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alfre\Dropbox (Personal)\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0B3C82-7414-4CE0-AE9B-A642009C2987}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2A8F673-15E6-4B1D-BFFE-31B24037D669}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{63F126C1-8083-4A20-9179-8C75EB50538A}"/>
   </bookViews>
@@ -57,7 +57,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,17 +90,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -405,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC0C28CD-24D2-4A4B-AA79-42D3E0783906}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,7 +427,7 @@
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -430,8 +440,15 @@
       <c r="D1">
         <v>29762</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G1">
+        <f>0.5306/0.984</f>
+        <v>0.53922764227642273</v>
+      </c>
+      <c r="J1">
+        <v>200.21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -444,11 +461,14 @@
       <c r="D2">
         <v>34988</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>-142.16999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -457,13 +477,28 @@
         <v>2.464442550960215E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="C5">
         <f>B1/(B1+B2)</f>
         <v>0.8734030197444832</v>
+      </c>
+      <c r="J5">
+        <v>58.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P6">
+        <f>12*5+10</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <f>1-29762/(29762+34988)</f>
+        <v>0.54035521235521233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>